<commit_message>
Inclusion of error rows in comparison file
</commit_message>
<xml_diff>
--- a/BIL_S1.xlsx
+++ b/BIL_S1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>TYPE</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>BIL</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
   <si>
     <t>E</t>
@@ -432,7 +435,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -446,10 +449,10 @@
         <v>123459</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -463,10 +466,10 @@
         <v>123458</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>